<commit_message>
revised from refreshed 80 pipeline
</commit_message>
<xml_diff>
--- a/ReportDefs_vervestacks.xlsx
+++ b/ReportDefs_vervestacks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids_syn_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFDB63D9-5188-4584-843D-9A4C3C9C035C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{60D44FBD-8237-45A3-907D-3013F81E10F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap_OLD" sheetId="70" r:id="rId1"/>
@@ -9316,7 +9316,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63B6CDE-608F-4316-9D2F-FCFA6B7BD309}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48167380-F8B3-49BF-B7F7-A1C29093D2FC}">
   <dimension ref="B9:H144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -12037,7 +12037,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F60CC30-FE94-4104-92A4-C51D85BE5EC9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C6DF58-A789-4FA9-8EC9-0A6FCEE3C29C}">
   <dimension ref="B9:L144"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>